<commit_message>
pulls out formulas, fails on no strings sheets
</commit_message>
<xml_diff>
--- a/test/spreadsheets/excel_mac_2011-basic.xlsx
+++ b/test/spreadsheets/excel_mac_2011-basic.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="19240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -36,14 +36,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,7 +77,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -398,24 +402,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1">
+        <f>SUM(D1:E1)</f>
+        <v>10</v>
+      </c>
+      <c r="D1">
+        <v>5</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -424,9 +438,10 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>